<commit_message>
Course Info, Excused Prereqs
</commit_message>
<xml_diff>
--- a/src/input_files/Course Info.xlsx
+++ b/src/input_files/Course Info.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\GitHub\scheduler\src\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679533C-3A34-4CF4-BACF-6C4D8C0AD86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4ACA7-E9A3-4C1D-8803-784DEC0FBB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="13350" windowHeight="8710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CPSC" sheetId="1" r:id="rId1"/>
+    <sheet name="ExcusedPrereqs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="181">
   <si>
     <t>courseID</t>
   </si>
@@ -425,18 +426,12 @@
     <t>CYBR 3106</t>
   </si>
   <si>
-    <t>CPSC 2106, CYBR 2160, CYBR 3128</t>
-  </si>
-  <si>
     <t>CYBR 3108</t>
   </si>
   <si>
     <t>Defensive Programming</t>
   </si>
   <si>
-    <t>CPSC 2106, CPSC 2108</t>
-  </si>
-  <si>
     <t>CYBR 3115</t>
   </si>
   <si>
@@ -449,9 +444,6 @@
     <t>Fundamentals of Digital Forensics</t>
   </si>
   <si>
-    <t>CPSC 2106, CYBR 2160</t>
-  </si>
-  <si>
     <t>CYBR 3126</t>
   </si>
   <si>
@@ -530,9 +522,6 @@
     <t>CYBR 4160</t>
   </si>
   <si>
-    <t>CPSC 2106, CPSC 2108, CYBR 2160</t>
-  </si>
-  <si>
     <t>CYBR 4166</t>
   </si>
   <si>
@@ -570,6 +559,24 @@
   </si>
   <si>
     <t>(4-0-4)</t>
+  </si>
+  <si>
+    <t>MISM 3145</t>
+  </si>
+  <si>
+    <t>MISM 3115</t>
+  </si>
+  <si>
+    <t>MISM 3109</t>
+  </si>
+  <si>
+    <t>CYBR 2160, CPSC 2108</t>
+  </si>
+  <si>
+    <t>CPSC 2108, CYBR 2160</t>
+  </si>
+  <si>
+    <t>CYBR 2160, CYBR 3128</t>
   </si>
 </sst>
 </file>
@@ -934,20 +941,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -979,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -996,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1013,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1036,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1096,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1133,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1153,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1173,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1193,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1253,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1273,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1293,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1313,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1333,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1370,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1424,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1444,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1467,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1510,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -1650,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -1670,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -1710,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1750,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -1770,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -1790,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -1847,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -1864,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -1881,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -1898,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -1918,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -1938,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -1952,18 +1959,18 @@
         <v>38</v>
       </c>
       <c r="E51" t="s">
+        <v>180</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>130</v>
       </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
         <v>131</v>
-      </c>
-      <c r="B52" t="s">
-        <v>132</v>
       </c>
       <c r="C52" t="s">
         <v>12</v>
@@ -1972,18 +1979,18 @@
         <v>32</v>
       </c>
       <c r="E52" t="s">
+        <v>178</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" t="s">
         <v>133</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>134</v>
-      </c>
-      <c r="B53" t="s">
-        <v>135</v>
       </c>
       <c r="C53" t="s">
         <v>12</v>
@@ -1998,12 +2005,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
         <v>12</v>
@@ -2012,18 +2019,18 @@
         <v>38</v>
       </c>
       <c r="E54" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
         <v>12</v>
@@ -2032,38 +2039,38 @@
         <v>32</v>
       </c>
       <c r="E55" t="s">
+        <v>138</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
         <v>141</v>
       </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="E56" t="s">
         <v>142</v>
       </c>
-      <c r="B56" t="s">
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" t="s">
         <v>143</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" t="s">
-        <v>145</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" t="s">
-        <v>146</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -2072,18 +2079,18 @@
         <v>38</v>
       </c>
       <c r="E57" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s">
         <v>12</v>
@@ -2092,35 +2099,35 @@
         <v>32</v>
       </c>
       <c r="E58" t="s">
+        <v>144</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>147</v>
       </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" t="s">
         <v>150</v>
-      </c>
-      <c r="B59" t="s">
-        <v>151</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" t="s">
-        <v>153</v>
       </c>
       <c r="C60" t="s">
         <v>12</v>
@@ -2129,18 +2136,18 @@
         <v>38</v>
       </c>
       <c r="E60" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
         <v>12</v>
@@ -2155,12 +2162,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
@@ -2175,12 +2182,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
         <v>12</v>
@@ -2195,12 +2202,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C64" t="s">
         <v>12</v>
@@ -2212,12 +2219,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -2232,9 +2239,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
         <v>124</v>
@@ -2246,18 +2253,18 @@
         <v>38</v>
       </c>
       <c r="E66" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -2272,15 +2279,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D68" t="s">
         <v>38</v>
@@ -2289,32 +2296,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
@@ -2329,12 +2336,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
@@ -2349,12 +2356,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B72" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
@@ -2370,4 +2377,44 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29CBC6-3612-40A0-A430-B8514E5BC998}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creation of Schedule Inspector to aid rules; updates to container, Path Excels, filter for directory batching
</commit_message>
<xml_diff>
--- a/src/input_files/Course Info.xlsx
+++ b/src/input_files/Course Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\GitHub\scheduler\src\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mel91\Desktop\lew\scheduler\src\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4ACA7-E9A3-4C1D-8803-784DEC0FBB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D789899A-C260-476B-AD1A-728326E95076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPSC" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="182">
   <si>
     <t>courseID</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>CYBR 2160, CYBR 3128</t>
+  </si>
+  <si>
+    <t>importance</t>
   </si>
 </sst>
 </file>
@@ -939,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +957,7 @@
     <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,8 +988,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1002,8 +1008,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1019,8 +1028,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1042,8 +1054,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1059,8 +1074,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1082,8 +1100,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1102,8 +1123,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1119,8 +1143,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1139,8 +1166,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1159,8 +1189,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1179,8 +1212,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1199,8 +1235,11 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1219,8 +1258,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1239,8 +1281,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1259,8 +1304,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1279,8 +1327,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1299,8 +1350,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1319,8 +1373,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1339,8 +1396,11 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1356,8 +1416,11 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1376,8 +1439,11 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1393,8 +1459,11 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1413,8 +1482,11 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1430,8 +1502,11 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1450,8 +1525,11 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1473,8 +1551,11 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1496,8 +1577,11 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1516,8 +1600,11 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -1536,8 +1623,11 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -1556,8 +1646,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K30">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1576,8 +1669,11 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1596,8 +1692,11 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -1616,8 +1715,11 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -1636,8 +1738,11 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -1656,8 +1761,11 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -1676,8 +1784,11 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -1696,8 +1807,11 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -1716,8 +1830,11 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -1736,8 +1853,11 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1756,8 +1876,11 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -1776,8 +1899,11 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -1796,8 +1922,11 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -1816,8 +1945,11 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -1833,8 +1965,11 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -1853,8 +1988,11 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -1870,8 +2008,11 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -1887,8 +2028,11 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -1904,8 +2048,11 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -1924,8 +2071,11 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -1944,8 +2094,11 @@
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -1964,8 +2117,11 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -1984,8 +2140,11 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -2004,8 +2163,11 @@
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>134</v>
       </c>
@@ -2024,8 +2186,11 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -2044,8 +2209,11 @@
       <c r="H55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>139</v>
       </c>
@@ -2064,8 +2232,11 @@
       <c r="H56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2084,8 +2255,11 @@
       <c r="H57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -2104,8 +2278,11 @@
       <c r="H58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>147</v>
       </c>
@@ -2121,8 +2298,11 @@
       <c r="H59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>149</v>
       </c>
@@ -2141,8 +2321,11 @@
       <c r="H60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>151</v>
       </c>
@@ -2161,8 +2344,11 @@
       <c r="H61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>153</v>
       </c>
@@ -2181,8 +2367,11 @@
       <c r="H62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>155</v>
       </c>
@@ -2201,8 +2390,11 @@
       <c r="H63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>157</v>
       </c>
@@ -2218,8 +2410,11 @@
       <c r="H64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>159</v>
       </c>
@@ -2238,8 +2433,11 @@
       <c r="H65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>161</v>
       </c>
@@ -2258,8 +2456,11 @@
       <c r="H66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>162</v>
       </c>
@@ -2278,8 +2479,11 @@
       <c r="H67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>164</v>
       </c>
@@ -2295,8 +2499,11 @@
       <c r="H68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2315,8 +2522,11 @@
       <c r="H69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K69">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -2335,8 +2545,11 @@
       <c r="H70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K70">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>170</v>
       </c>
@@ -2355,8 +2568,11 @@
       <c r="H71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K71">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>172</v>
       </c>
@@ -2371,6 +2587,9 @@
       </c>
       <c r="H72">
         <v>0</v>
+      </c>
+      <c r="K72">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2383,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29CBC6-3612-40A0-A430-B8514E5BC998}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Course Info Container Update along w/connected modules' relations to it
</commit_message>
<xml_diff>
--- a/src/input_files/Course Info.xlsx
+++ b/src/input_files/Course Info.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mel91\Desktop\lew\scheduler\src\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D789899A-C260-476B-AD1A-728326E95076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C932E834-0D74-49F3-B3D3-EF6FC7DA3D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPSC" sheetId="1" r:id="rId1"/>
-    <sheet name="ExcusedPrereqs" sheetId="2" r:id="rId2"/>
+    <sheet name="CYBR" sheetId="3" r:id="rId2"/>
+    <sheet name="MATH" sheetId="4" r:id="rId3"/>
+    <sheet name="ExcusedPrereqs" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="182">
   <si>
     <t>courseID</t>
   </si>
@@ -942,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,541 +2056,21 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="K49">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" t="s">
-        <v>125</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" t="s">
-        <v>38</v>
-      </c>
-      <c r="E51" t="s">
-        <v>180</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" t="s">
-        <v>178</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>132</v>
-      </c>
-      <c r="B53" t="s">
-        <v>133</v>
-      </c>
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>134</v>
-      </c>
-      <c r="B54" t="s">
-        <v>135</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="K54">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>136</v>
-      </c>
-      <c r="B55" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" t="s">
-        <v>138</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>139</v>
-      </c>
-      <c r="B56" t="s">
-        <v>140</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" t="s">
-        <v>141</v>
-      </c>
-      <c r="E56" t="s">
-        <v>142</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" t="s">
-        <v>143</v>
-      </c>
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" t="s">
-        <v>144</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>145</v>
-      </c>
-      <c r="B58" t="s">
-        <v>146</v>
-      </c>
-      <c r="C58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" t="s">
-        <v>144</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>147</v>
-      </c>
-      <c r="B59" t="s">
-        <v>148</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>149</v>
-      </c>
-      <c r="B60" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" t="s">
-        <v>127</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
-        <v>127</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62" t="s">
-        <v>154</v>
-      </c>
-      <c r="C62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" t="s">
-        <v>127</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>155</v>
-      </c>
-      <c r="B63" t="s">
-        <v>156</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E63" t="s">
-        <v>127</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" t="s">
-        <v>158</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" t="s">
-        <v>38</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" t="s">
-        <v>160</v>
-      </c>
-      <c r="C65" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" t="s">
-        <v>127</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>161</v>
-      </c>
-      <c r="B66" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" t="s">
-        <v>38</v>
-      </c>
-      <c r="E66" t="s">
-        <v>179</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="K66">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>162</v>
-      </c>
-      <c r="B67" t="s">
-        <v>163</v>
-      </c>
-      <c r="C67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" t="s">
-        <v>38</v>
-      </c>
-      <c r="E67" t="s">
-        <v>88</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" t="s">
-        <v>165</v>
-      </c>
-      <c r="C68" t="s">
-        <v>166</v>
-      </c>
-      <c r="D68" t="s">
-        <v>38</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" t="s">
-        <v>167</v>
-      </c>
-      <c r="C69" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" t="s">
-        <v>168</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="K69">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" t="s">
-        <v>169</v>
-      </c>
-      <c r="C70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" t="s">
-        <v>19</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>170</v>
-      </c>
-      <c r="B71" t="s">
-        <v>171</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" t="s">
-        <v>26</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="K71">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>172</v>
-      </c>
-      <c r="B72" t="s">
-        <v>173</v>
-      </c>
-      <c r="C72" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="K72">
         <v>50</v>
       </c>
     </row>
@@ -2599,6 +2081,640 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1230F2EE-D5F0-4670-B252-10EC0E3FCD5B}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0197F54C-D26E-487D-9FAF-620401D35907}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29CBC6-3612-40A0-A430-B8514E5BC998}">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>